<commit_message>
Website was updated so change the Code
</commit_message>
<xml_diff>
--- a/TestCase-AllPosters.xlsx
+++ b/TestCase-AllPosters.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="183">
   <si>
     <r>
       <rPr>
@@ -194,14 +194,7 @@
     <t>Login Module</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Login using valid credentials</t>
-    </r>
+    <t>Positive Login Scenario</t>
   </si>
   <si>
     <t>Enter valid email and password</t>
@@ -229,24 +222,10 @@
     <t>High</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1F1F1F"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>User should be navigated to dashboard</t>
-    </r>
+    <t>User is navigated to dashboard</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Click on login and user should be navigated to dashboard</t>
-    </r>
+    <t>User should be navigated to dashboard</t>
   </si>
   <si>
     <r>
@@ -272,6 +251,10 @@
     </r>
   </si>
   <si>
+    <t>Chromium 124,
+Windows 11</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -292,14 +275,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Login using invalid credentials</t>
-    </r>
+    <t>Negative Login Scenario</t>
   </si>
   <si>
     <t>Enter invalid email and invalid password</t>
@@ -324,20 +300,10 @@
     <t>url: www.allposters.com email: admin@test.com password: admin</t>
   </si>
   <si>
-    <t>Medium</t>
+    <t>Error message is displayed</t>
   </si>
   <si>
-    <t>Invalid email or password displayed</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Click on login and error message should be displayed</t>
-    </r>
+    <t xml:space="preserve"> 'Incorrect username or password, please try again.' message should be displayed</t>
   </si>
   <si>
     <r>
@@ -380,16 +346,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Login using invalid credentials</t>
-    </r>
-  </si>
-  <si>
     <t>Enter valid email and invalid password</t>
   </si>
   <si>
@@ -410,16 +366,6 @@
   </si>
   <si>
     <t>url: www.allposters.com email: rojal2002@gmail.com password: test123</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Click on login and error message should be displayed</t>
-    </r>
   </si>
   <si>
     <r>
@@ -462,9 +408,6 @@
     </r>
   </si>
   <si>
-    <t>Login using invalid credentials</t>
-  </si>
-  <si>
     <t>Enter invalid email and valid password</t>
   </si>
   <si>
@@ -485,16 +428,6 @@
   </si>
   <si>
     <t>url: www.allposters.com email: admin@test.com password: Rojalposters@10</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Click on login and error message should be displayed</t>
-    </r>
   </si>
   <si>
     <r>
@@ -537,16 +470,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Login using empty credentials</t>
-    </r>
-  </si>
-  <si>
     <t>Enter empty email and valid password</t>
   </si>
   <si>
@@ -570,14 +493,7 @@
 password: Rojalposters@11</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Click on login and error message should be displayed</t>
-    </r>
+    <t xml:space="preserve"> 'Please enter your email address.' message should be displayed</t>
   </si>
   <si>
     <r>
@@ -620,16 +536,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Login using empty credentials</t>
-    </r>
-  </si>
-  <si>
     <t>Enter empty password and valid email</t>
   </si>
   <si>
@@ -653,17 +559,7 @@
 password: </t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Click on login and error message should be displayed</t>
-    </r>
+    <t xml:space="preserve"> 'Please enter your password.' message should be displayed</t>
   </si>
   <si>
     <r>
@@ -706,27 +602,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Login using empty credentials</t>
-    </r>
-  </si>
-  <si>
     <t>Enter empty email and invalid password</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>System must be up and running</t>
-    </r>
+    <t>System must be up and running</t>
   </si>
   <si>
     <t>1. Open specified url
@@ -737,16 +616,6 @@
   <si>
     <t>url: www.allposters.com email:  
 password: test123</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Click on login and error message should be displayed</t>
-    </r>
   </si>
   <si>
     <r>
@@ -789,27 +658,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Login using empty credentials</t>
-    </r>
-  </si>
-  <si>
     <t>Enter empty password and invalid email</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>System must be up and running</t>
-    </r>
   </si>
   <si>
     <t>1. Open specified url
@@ -820,16 +669,6 @@
   <si>
     <t xml:space="preserve">url: www.allposters.com email: root@gmail.com 
 password: </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Click on login and error message should be displayed</t>
-    </r>
   </si>
   <si>
     <r>
@@ -878,16 +717,6 @@
         <color theme="1"/>
         <sz val="11.0"/>
       </rPr>
-      <t>Login using empty credentials</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
       <t>Empty username and password</t>
     </r>
   </si>
@@ -912,24 +741,10 @@
 password: </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Click on login and error message should be displayed</t>
-    </r>
+    <t xml:space="preserve"> 'Please enter your email address. Please enter your password. 'message should be displayed</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>User gets error message and redirected to login page</t>
-    </r>
+    <t>User gets error message and redirected to login page</t>
   </si>
   <si>
     <r>
@@ -958,14 +773,14 @@
     <t>Search Module</t>
   </si>
   <si>
-    <t>Valid Search Functionality</t>
+    <t>Positive Search Scenario</t>
   </si>
   <si>
     <t>Search with valid term</t>
   </si>
   <si>
-    <t>Website must be up and running and user 
-must be on the search page</t>
+    <t>Website must be up and running
+and user must be on the search page</t>
   </si>
   <si>
     <t>1. Open specified url
@@ -979,10 +794,10 @@
 </t>
   </si>
   <si>
-    <t>User sees search results</t>
+    <t>Search result page is updated to show posters</t>
   </si>
   <si>
-    <t>Press Enter and the search results should be displayed</t>
+    <t>The search results should be displayed</t>
   </si>
   <si>
     <t>The search results are displayed as expected</t>
@@ -1004,7 +819,7 @@
     <t>Search_002</t>
   </si>
   <si>
-    <t>Invalid Search Functionality</t>
+    <t>Negative Search Scenario</t>
   </si>
   <si>
     <t>Search with invalid term (random string)</t>
@@ -1021,13 +836,19 @@
 </t>
   </si>
   <si>
-    <t>User sees no search results</t>
+    <t>The page shows 'Uh oh! Looks like something 
+went wrong on our end.Please try again later, 
+or head back to the homepage' message</t>
   </si>
   <si>
-    <t>Press Enter and the error message should be displayed</t>
+    <t xml:space="preserve"> 'Uh oh! Looks like something 
+went wrong on our end.Please try again later, 
+or head back to the homepage' message should be displayed</t>
   </si>
   <si>
-    <t>User gets error message indicating 'Please try again later'</t>
+    <t xml:space="preserve"> 'Uh oh! Looks like something 
+went wrong on our end.Please try again later, 
+or head back to the homepage' message is displayed</t>
   </si>
   <si>
     <t>Test successful error message is displayed</t>
@@ -1060,7 +881,12 @@
 </t>
   </si>
   <si>
-    <t>Press Enter and nothing should be displayed</t>
+    <t>The page does not update, and no search is 
+performed</t>
+  </si>
+  <si>
+    <t>The page should remain unchanged with no search results 
+displayed</t>
   </si>
   <si>
     <t>No message is displayed</t>
@@ -1094,6 +920,16 @@
     <t xml:space="preserve">url: www.allposters.com 
 search: :':%%^&amp;
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Uh oh! Looks like something 
+went wrong on our end.Please try again later, 
+or head back to the homepage' message should be displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Uh oh! Looks like something 
+went wrong on our end.Please try again later, 
+or head back to the homepage' message is displayed</t>
   </si>
   <si>
     <r>
@@ -1168,14 +1004,14 @@
     <t>Logout Module</t>
   </si>
   <si>
-    <t>User successfully logs out of the system</t>
+    <t>Positive Logout Scenario</t>
   </si>
   <si>
     <t xml:space="preserve">Click Logout </t>
   </si>
   <si>
-    <t>Website must be up and running and user 
-must be logged in</t>
+    <t>Website must be up and running and
+user must be logged in</t>
   </si>
   <si>
     <t>1. Navigate to login page
@@ -1222,9 +1058,6 @@
     <t>Logout_002</t>
   </si>
   <si>
-    <t>Session termination check</t>
-  </si>
-  <si>
     <t>Verify that the session terminates upon logout</t>
   </si>
   <si>
@@ -1266,12 +1099,78 @@
       <t>(screenshot and copy url)</t>
     </r>
   </si>
+  <si>
+    <t>Cart_001</t>
+  </si>
+  <si>
+    <t>Cart Module</t>
+  </si>
+  <si>
+    <t>Positive AddtoCart Scenario</t>
+  </si>
+  <si>
+    <t>Add product to the cart</t>
+  </si>
+  <si>
+    <t>1. Open specified url
+2. Login
+3. Search 
+4. Add product to cart</t>
+  </si>
+  <si>
+    <t>Product should be added to the cart</t>
+  </si>
+  <si>
+    <t>Product is added to the cart</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>(screenshot and copy url)</t>
+    </r>
+  </si>
+  <si>
+    <t>Cart_002</t>
+  </si>
+  <si>
+    <t>Postive RemovetoCart Scenario</t>
+  </si>
+  <si>
+    <t>Remove product from the cart</t>
+  </si>
+  <si>
+    <t>1. Open specified url
+2. Login
+3. Search 
+4. Add product to cart
+5. Remove product from cart</t>
+  </si>
+  <si>
+    <t>Product should be removed from the cart</t>
+  </si>
+  <si>
+    <t>Product is removed from the cart</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>(screenshot and copy url)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1300,8 +1199,13 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1314,6 +1218,12 @@
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -1321,7 +1231,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
@@ -1349,17 +1259,20 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1584,12 +1497,12 @@
     <col customWidth="1" min="2" max="2" width="16.57"/>
     <col customWidth="1" min="3" max="3" width="42.43"/>
     <col customWidth="1" min="4" max="4" width="47.43"/>
-    <col customWidth="1" min="5" max="5" width="40.14"/>
+    <col customWidth="1" min="5" max="5" width="36.57"/>
     <col customWidth="1" min="6" max="6" width="37.29"/>
     <col customWidth="1" min="7" max="7" width="28.57"/>
     <col customWidth="1" min="8" max="8" width="15.57"/>
     <col customWidth="1" min="9" max="9" width="14.43"/>
-    <col customWidth="1" min="10" max="10" width="39.29"/>
+    <col customWidth="1" min="10" max="10" width="44.29"/>
     <col customWidth="1" min="11" max="11" width="58.71"/>
     <col customWidth="1" min="12" max="12" width="56.57"/>
     <col customWidth="1" min="13" max="13" width="13.0"/>
@@ -1665,7 +1578,7 @@
       <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -1686,10 +1599,10 @@
       <c r="I2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>25</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -1701,9 +1614,11 @@
       <c r="N2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="9"/>
+      <c r="O2" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="P2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -1718,33 +1633,33 @@
     </row>
     <row r="3" ht="60.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="H3" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="I3" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="5" t="s">
         <v>38</v>
       </c>
       <c r="L3" s="3" t="s">
@@ -1756,7 +1671,6 @@
       <c r="N3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="9"/>
       <c r="P3" s="3" t="s">
         <v>41</v>
       </c>
@@ -1775,45 +1689,41 @@
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="H4" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>48</v>
+      <c r="K4" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>27</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
-      <c r="O4" s="9"/>
       <c r="P4" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
@@ -1828,22 +1738,19 @@
     </row>
     <row r="5" ht="56.25" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="F5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="G5" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>23</v>
@@ -1854,21 +1761,20 @@
       <c r="J5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>58</v>
+      <c r="K5" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>27</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
-      <c r="O5" s="9"/>
       <c r="P5" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -1883,22 +1789,19 @@
     </row>
     <row r="6" ht="55.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>23</v>
@@ -1909,21 +1812,20 @@
       <c r="J6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>68</v>
+      <c r="K6" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
-      <c r="O6" s="9"/>
       <c r="P6" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
@@ -1938,47 +1840,43 @@
     </row>
     <row r="7" ht="56.25" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>79</v>
+      <c r="K7" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>27</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
-      <c r="O7" s="9"/>
       <c r="P7" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -1993,22 +1891,19 @@
     </row>
     <row r="8" ht="55.5" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>86</v>
+      <c r="E8" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>23</v>
@@ -2019,21 +1914,20 @@
       <c r="J8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>89</v>
+      <c r="K8" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="M8" s="8" t="s">
         <v>27</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
-      <c r="O8" s="9"/>
       <c r="P8" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -2048,22 +1942,19 @@
     </row>
     <row r="9" ht="58.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>96</v>
+      <c r="E9" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>23</v>
@@ -2074,21 +1965,20 @@
       <c r="J9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>99</v>
+      <c r="K9" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="M9" s="8" t="s">
         <v>27</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
-      <c r="O9" s="9"/>
       <c r="P9" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -2103,22 +1993,19 @@
     </row>
     <row r="10" ht="57.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>23</v>
@@ -2129,21 +2016,20 @@
       <c r="J10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>109</v>
+      <c r="K10" s="5" t="s">
+        <v>96</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>110</v>
+      <c r="L10" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>27</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
-      <c r="O10" s="9"/>
       <c r="P10" s="3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -2158,25 +2044,25 @@
     </row>
     <row r="11" ht="64.5" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>23</v>
@@ -2185,23 +2071,22 @@
         <v>23</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="M11" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
-      <c r="O11" s="11"/>
       <c r="P11" s="3" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -2216,22 +2101,22 @@
     </row>
     <row r="12" ht="65.25" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>23</v>
@@ -2240,23 +2125,22 @@
         <v>23</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="M12" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
-      <c r="O12" s="11"/>
       <c r="P12" s="3" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -2271,22 +2155,19 @@
     </row>
     <row r="13" ht="70.5" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>23</v>
@@ -2295,23 +2176,22 @@
         <v>23</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="M13" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
-      <c r="O13" s="2"/>
       <c r="P13" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -2326,22 +2206,19 @@
     </row>
     <row r="14" ht="67.5" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>23</v>
@@ -2350,23 +2227,22 @@
         <v>23</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="M14" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
-      <c r="O14" s="2"/>
       <c r="P14" s="3" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -2381,22 +2257,19 @@
     </row>
     <row r="15" ht="77.25" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>23</v>
@@ -2405,23 +2278,22 @@
         <v>23</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="M15" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
-      <c r="O15" s="2"/>
       <c r="P15" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -2436,22 +2308,22 @@
     </row>
     <row r="16" ht="72.75" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>23</v>
@@ -2460,23 +2332,22 @@
         <v>23</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="M16" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
-      <c r="O16" s="2"/>
       <c r="P16" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -2491,25 +2362,25 @@
     </row>
     <row r="17" ht="127.5" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>163</v>
+      <c r="F17" s="11" t="s">
+        <v>153</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>23</v>
@@ -2518,23 +2389,22 @@
         <v>23</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="M17" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
-      <c r="O17" s="2"/>
       <c r="P17" s="3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -2549,22 +2419,19 @@
     </row>
     <row r="18" ht="152.25" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="E18" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="F18" s="12" t="s">
-        <v>173</v>
-      </c>
       <c r="G18" s="7" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>23</v>
@@ -2573,23 +2440,22 @@
         <v>23</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="M18" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
-      <c r="O18" s="2"/>
       <c r="P18" s="3" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -2603,22 +2469,49 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
+      <c r="A19" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -2631,22 +2524,46 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
+      <c r="A20" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="G20" s="13"/>
+      <c r="H20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
@@ -30099,16 +30016,21 @@
       <c r="Z1000" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
     <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C3:C10"/>
     <mergeCell ref="B11:B16"/>
+    <mergeCell ref="C12:C15"/>
     <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="O2:O20"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M2:M18">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M2:M20">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:I18">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:I20">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>